<commit_message>
library cleanup + added and tested PyScripts
</commit_message>
<xml_diff>
--- a/PyScripts/output/std_day.xlsx
+++ b/PyScripts/output/std_day.xlsx
@@ -472,34 +472,34 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>36805.6034055525</v>
+        <v>36373.28826856845</v>
       </c>
       <c r="C2" t="n">
-        <v>33628.60106608918</v>
+        <v>32828.32581981639</v>
       </c>
       <c r="D2" t="n">
-        <v>33936.65516706211</v>
+        <v>33111.22475746145</v>
       </c>
       <c r="E2" t="n">
-        <v>34278.77687429454</v>
+        <v>33427.38324280769</v>
       </c>
       <c r="F2" t="n">
-        <v>34652.96936729366</v>
+        <v>33774.83582826793</v>
       </c>
       <c r="G2" t="n">
-        <v>34868.06168990825</v>
+        <v>33963.38123296577</v>
       </c>
       <c r="H2" t="n">
-        <v>34816.40257494969</v>
+        <v>33886.06427502663</v>
       </c>
       <c r="I2" t="n">
-        <v>34774.87764196407</v>
+        <v>33818.51708178314</v>
       </c>
       <c r="J2" t="n">
-        <v>33768.54388465991</v>
+        <v>32766.82248902799</v>
       </c>
       <c r="K2" t="n">
-        <v>29461.81254154599</v>
+        <v>28689.97216651863</v>
       </c>
     </row>
     <row r="3">
@@ -509,34 +509,34 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>28872.74105241501</v>
+        <v>28644.23911667487</v>
       </c>
       <c r="C3" t="n">
-        <v>25874.7184173299</v>
+        <v>25437.85421204317</v>
       </c>
       <c r="D3" t="n">
-        <v>25810.40715673481</v>
+        <v>25372.37373150306</v>
       </c>
       <c r="E3" t="n">
-        <v>25759.69842691205</v>
+        <v>25320.62365315176</v>
       </c>
       <c r="F3" t="n">
-        <v>25721.79526650354</v>
+        <v>25281.80043190278</v>
       </c>
       <c r="G3" t="n">
-        <v>25571.06949134485</v>
+        <v>25130.52850649365</v>
       </c>
       <c r="H3" t="n">
-        <v>25237.19482766133</v>
+        <v>24796.61272205292</v>
       </c>
       <c r="I3" t="n">
-        <v>24903.7724266241</v>
+        <v>24463.25406783813</v>
       </c>
       <c r="J3" t="n">
-        <v>23581.92279390812</v>
+        <v>23146.60140917578</v>
       </c>
       <c r="K3" t="n">
-        <v>23554.7701728358</v>
+        <v>23125.19029400865</v>
       </c>
     </row>
     <row r="4">
@@ -546,34 +546,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>28604.99110218415</v>
+        <v>28159.8542017977</v>
       </c>
       <c r="C4" t="n">
-        <v>28609.19124825222</v>
+        <v>28159.8542017977</v>
       </c>
       <c r="D4" t="n">
-        <v>28610.36711707896</v>
+        <v>28159.8542017977</v>
       </c>
       <c r="E4" t="n">
-        <v>28611.48419385804</v>
+        <v>28159.8542017977</v>
       </c>
       <c r="F4" t="n">
-        <v>28612.54434176847</v>
+        <v>28159.8542017977</v>
       </c>
       <c r="G4" t="n">
-        <v>28613.54942318858</v>
+        <v>28159.8542017977</v>
       </c>
       <c r="H4" t="n">
-        <v>28614.50130591325</v>
+        <v>28159.8542017977</v>
       </c>
       <c r="I4" t="n">
-        <v>28615.40187021191</v>
+        <v>28159.8542017977</v>
       </c>
       <c r="J4" t="n">
-        <v>28617.16071002089</v>
+        <v>28159.8542017977</v>
       </c>
       <c r="K4" t="n">
-        <v>28611.31659759762</v>
+        <v>28159.8542017977</v>
       </c>
     </row>
     <row r="5">
@@ -583,34 +583,34 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>267.7499502308674</v>
+        <v>484.3849148771696</v>
       </c>
       <c r="C5" t="n">
-        <v>-2734.472830922321</v>
+        <v>-2721.999989754528</v>
       </c>
       <c r="D5" t="n">
-        <v>-2799.959960344149</v>
+        <v>-2787.480470294639</v>
       </c>
       <c r="E5" t="n">
-        <v>-2851.785766945988</v>
+        <v>-2839.230548645945</v>
       </c>
       <c r="F5" t="n">
-        <v>-2890.749075264932</v>
+        <v>-2878.053769894919</v>
       </c>
       <c r="G5" t="n">
-        <v>-3042.479931843733</v>
+        <v>-3029.325695304055</v>
       </c>
       <c r="H5" t="n">
-        <v>-3377.306478251925</v>
+        <v>-3363.241479744785</v>
       </c>
       <c r="I5" t="n">
-        <v>-3711.629443587815</v>
+        <v>-3696.600133959575</v>
       </c>
       <c r="J5" t="n">
-        <v>-5035.237916112776</v>
+        <v>-5013.252792621915</v>
       </c>
       <c r="K5" t="n">
-        <v>-5056.546424761826</v>
+        <v>-5034.66390778905</v>
       </c>
     </row>
     <row r="6">
@@ -620,34 +620,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1657.518489434291</v>
+        <v>1681.227758686155</v>
       </c>
       <c r="C6" t="n">
-        <v>1085.252874909611</v>
+        <v>1081.420427045613</v>
       </c>
       <c r="D6" t="n">
-        <v>1073.18066485897</v>
+        <v>1069.294750926665</v>
       </c>
       <c r="E6" t="n">
-        <v>1063.647690722715</v>
+        <v>1059.723614166635</v>
       </c>
       <c r="F6" t="n">
-        <v>1056.510661022054</v>
+        <v>1052.562796005634</v>
       </c>
       <c r="G6" t="n">
-        <v>1028.478596636709</v>
+        <v>1024.515715959518</v>
       </c>
       <c r="H6" t="n">
-        <v>966.5513245764751</v>
+        <v>962.5784025424464</v>
       </c>
       <c r="I6" t="n">
-        <v>904.7607402322701</v>
+        <v>900.7873297381775</v>
       </c>
       <c r="J6" t="n">
-        <v>654.8626793539888</v>
+        <v>651.5398652914637</v>
       </c>
       <c r="K6" t="n">
-        <v>639.9360041528453</v>
+        <v>637.3431019090867</v>
       </c>
     </row>
     <row r="7">
@@ -657,34 +657,34 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1576.305828747898</v>
+        <v>1567.5</v>
       </c>
       <c r="C7" t="n">
-        <v>1576.345811213993</v>
+        <v>1567.5</v>
       </c>
       <c r="D7" t="n">
-        <v>1576.356096690382</v>
+        <v>1567.5</v>
       </c>
       <c r="E7" t="n">
-        <v>1576.365845787418</v>
+        <v>1567.5</v>
       </c>
       <c r="F7" t="n">
-        <v>1576.375076067036</v>
+        <v>1567.5</v>
       </c>
       <c r="G7" t="n">
-        <v>1576.384050802064</v>
+        <v>1567.5</v>
       </c>
       <c r="H7" t="n">
-        <v>1576.392926080014</v>
+        <v>1567.5</v>
       </c>
       <c r="I7" t="n">
-        <v>1576.401358239893</v>
+        <v>1567.5</v>
       </c>
       <c r="J7" t="n">
-        <v>1576.418317606475</v>
+        <v>1567.5</v>
       </c>
       <c r="K7" t="n">
-        <v>1576.372330214937</v>
+        <v>1567.5</v>
       </c>
     </row>
     <row r="8">
@@ -694,34 +694,34 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>81.21266068639397</v>
+        <v>113.7277586861551</v>
       </c>
       <c r="C8" t="n">
-        <v>-491.0929363043815</v>
+        <v>-486.079572954387</v>
       </c>
       <c r="D8" t="n">
-        <v>-503.1754318314124</v>
+        <v>-498.2052490733349</v>
       </c>
       <c r="E8" t="n">
-        <v>-512.7181550647028</v>
+        <v>-507.7763858333647</v>
       </c>
       <c r="F8" t="n">
-        <v>-519.8644150449823</v>
+        <v>-514.9372039943664</v>
       </c>
       <c r="G8" t="n">
-        <v>-547.9054541653545</v>
+        <v>-542.9842840404817</v>
       </c>
       <c r="H8" t="n">
-        <v>-609.8416015035391</v>
+        <v>-604.9215974575536</v>
       </c>
       <c r="I8" t="n">
-        <v>-671.6406180076233</v>
+        <v>-666.7126702618225</v>
       </c>
       <c r="J8" t="n">
-        <v>-921.5556382524865</v>
+        <v>-915.9601347085363</v>
       </c>
       <c r="K8" t="n">
-        <v>-936.4363260620919</v>
+        <v>-930.1568980909133</v>
       </c>
     </row>
     <row r="9">
@@ -731,34 +731,34 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-5.873785400390602</v>
+        <v>-5.451086425781227</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.887274169921852</v>
+        <v>-1.165106201171852</v>
       </c>
       <c r="D9" t="n">
-        <v>-2.168981933593727</v>
+        <v>-1.423010253906227</v>
       </c>
       <c r="E9" t="n">
-        <v>-2.481176757812477</v>
+        <v>-1.710668945312477</v>
       </c>
       <c r="F9" t="n">
-        <v>-2.822088623046852</v>
+        <v>-2.026281738281227</v>
       </c>
       <c r="G9" t="n">
-        <v>-3.035559082031227</v>
+        <v>-2.214483642578102</v>
       </c>
       <c r="H9" t="n">
-        <v>-3.033697509765602</v>
+        <v>-2.187811279296852</v>
       </c>
       <c r="I9" t="n">
-        <v>-3.042211914062477</v>
+        <v>-2.171179199218727</v>
       </c>
       <c r="J9" t="n">
-        <v>-2.357153320312477</v>
+        <v>-1.440283203124977</v>
       </c>
       <c r="K9" t="n">
-        <v>-3.021826171874977</v>
+        <v>-2.182440185546852</v>
       </c>
     </row>
     <row r="10">
@@ -768,34 +768,34 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>23.99430379406022</v>
+        <v>23.84453740855605</v>
       </c>
       <c r="C10" t="n">
-        <v>24.08561372784669</v>
+        <v>23.98732364919283</v>
       </c>
       <c r="D10" t="n">
-        <v>24.08390299010432</v>
+        <v>23.98801190270962</v>
       </c>
       <c r="E10" t="n">
-        <v>24.08517723456424</v>
+        <v>23.99132867835647</v>
       </c>
       <c r="F10" t="n">
-        <v>24.08928932611661</v>
+        <v>23.99714815349495</v>
       </c>
       <c r="G10" t="n">
-        <v>24.06033181884544</v>
+        <v>23.97237388782048</v>
       </c>
       <c r="H10" t="n">
-        <v>23.97814665312694</v>
+        <v>23.89839661419558</v>
       </c>
       <c r="I10" t="n">
-        <v>23.89522322313161</v>
+        <v>23.82359664696867</v>
       </c>
       <c r="J10" t="n">
-        <v>23.83972692369031</v>
+        <v>23.791955280438</v>
       </c>
       <c r="K10" t="n">
-        <v>24.07429568413727</v>
+        <v>24.00619918249913</v>
       </c>
     </row>
     <row r="11">
@@ -805,34 +805,34 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>23.99999999999216</v>
+        <v>24.00000000004019</v>
       </c>
       <c r="C11" t="n">
-        <v>23.99999999999983</v>
+        <v>23.9999999998825</v>
       </c>
       <c r="D11" t="n">
-        <v>23.99999999999994</v>
+        <v>23.99999999999557</v>
       </c>
       <c r="E11" t="n">
-        <v>24.00000000000006</v>
+        <v>23.99999999999926</v>
       </c>
       <c r="F11" t="n">
         <v>23.99999999999983</v>
       </c>
       <c r="G11" t="n">
-        <v>24.00000000000006</v>
+        <v>23.9999999999996</v>
       </c>
       <c r="H11" t="n">
-        <v>24.00000000000023</v>
+        <v>23.99999999999972</v>
       </c>
       <c r="I11" t="n">
-        <v>24.00000000000034</v>
+        <v>23.99999999999977</v>
       </c>
       <c r="J11" t="n">
-        <v>23.99999999999812</v>
+        <v>23.99999999999983</v>
       </c>
       <c r="K11" t="n">
-        <v>23.99999999999983</v>
+        <v>23.99999999995293</v>
       </c>
     </row>
     <row r="12">
@@ -842,34 +842,34 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>24.07408995683602</v>
+        <v>24.10240300547554</v>
       </c>
       <c r="C12" t="n">
-        <v>23.58116990223107</v>
+        <v>23.58161050234139</v>
       </c>
       <c r="D12" t="n">
-        <v>23.57150741463425</v>
+        <v>23.57192269146827</v>
       </c>
       <c r="E12" t="n">
-        <v>23.56377790707546</v>
+        <v>23.56418304479172</v>
       </c>
       <c r="F12" t="n">
-        <v>23.55785747811075</v>
+        <v>23.5582666181997</v>
       </c>
       <c r="G12" t="n">
-        <v>23.53637549681338</v>
+        <v>23.53678143226557</v>
       </c>
       <c r="H12" t="n">
-        <v>23.48955816112317</v>
+        <v>23.4899411607214</v>
       </c>
       <c r="I12" t="n">
-        <v>23.44280070477356</v>
+        <v>23.44316849016877</v>
       </c>
       <c r="J12" t="n">
-        <v>23.25666113520236</v>
+        <v>23.25738205723979</v>
       </c>
       <c r="K12" t="n">
-        <v>23.12114425430354</v>
+        <v>23.12202466584654</v>
       </c>
     </row>
     <row r="13">
@@ -879,34 +879,34 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>24.13990410382553</v>
+        <v>24.04445599188716</v>
       </c>
       <c r="C13" t="n">
-        <v>23.26237528466066</v>
+        <v>23.18810105603154</v>
       </c>
       <c r="D13" t="n">
-        <v>23.24116182140421</v>
+        <v>23.16961254466679</v>
       </c>
       <c r="E13" t="n">
-        <v>23.22665621466308</v>
+        <v>23.15742066529475</v>
       </c>
       <c r="F13" t="n">
-        <v>23.21847983343707</v>
+        <v>23.15117223160536</v>
       </c>
       <c r="G13" t="n">
-        <v>23.14751594889071</v>
+        <v>23.08527498221935</v>
       </c>
       <c r="H13" t="n">
-        <v>22.9748527812668</v>
+        <v>22.92276118539974</v>
       </c>
       <c r="I13" t="n">
-        <v>22.80151834851767</v>
+        <v>22.75949828507527</v>
       </c>
       <c r="J13" t="n">
-        <v>22.38466744652118</v>
+        <v>22.37520044139393</v>
       </c>
       <c r="K13" t="n">
-        <v>22.4019674074799</v>
+        <v>22.37694212082602</v>
       </c>
     </row>
     <row r="14">
@@ -916,34 +916,34 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>12.16520004504747</v>
+        <v>12.23839114264644</v>
       </c>
       <c r="C14" t="n">
-        <v>14.4452929954183</v>
+        <v>14.6305321978881</v>
       </c>
       <c r="D14" t="n">
-        <v>14.49043646790261</v>
+        <v>14.67646779989116</v>
       </c>
       <c r="E14" t="n">
-        <v>14.52786784897211</v>
+        <v>14.71459397409853</v>
       </c>
       <c r="F14" t="n">
-        <v>14.55802616364844</v>
+        <v>14.74535530375152</v>
       </c>
       <c r="G14" t="n">
-        <v>14.64675709578916</v>
+        <v>14.83469630730582</v>
       </c>
       <c r="H14" t="n">
-        <v>14.8309102211652</v>
+        <v>15.01952440727166</v>
       </c>
       <c r="I14" t="n">
-        <v>15.01429785861461</v>
+        <v>15.20352381637599</v>
       </c>
       <c r="J14" t="n">
-        <v>15.72364413771135</v>
+        <v>15.91260021927872</v>
       </c>
       <c r="K14" t="n">
-        <v>13.98935515919248</v>
+        <v>14.21063626146469</v>
       </c>
     </row>
     <row r="15">
@@ -953,34 +953,34 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>9.180975342448416</v>
+        <v>9.212165898480206</v>
       </c>
       <c r="C15" t="n">
-        <v>8.160626439361495</v>
+        <v>8.166351844817301</v>
       </c>
       <c r="D15" t="n">
-        <v>7.915996718284249</v>
+        <v>7.920414662332316</v>
       </c>
       <c r="E15" t="n">
-        <v>7.682265473915666</v>
+        <v>7.685613563694098</v>
       </c>
       <c r="F15" t="n">
-        <v>7.459224660221128</v>
+        <v>7.461712185378011</v>
       </c>
       <c r="G15" t="n">
-        <v>7.26225656555454</v>
+        <v>7.262864872021299</v>
       </c>
       <c r="H15" t="n">
-        <v>7.098463280745038</v>
+        <v>7.095582782537317</v>
       </c>
       <c r="I15" t="n">
-        <v>6.944057504201787</v>
+        <v>6.937872541435467</v>
       </c>
       <c r="J15" t="n">
-        <v>6.565468881857826</v>
+        <v>6.550943243122166</v>
       </c>
       <c r="K15" t="n">
-        <v>7.534060563228241</v>
+        <v>7.52642136078125</v>
       </c>
     </row>
     <row r="16">
@@ -990,34 +990,34 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17.32258285775677</v>
+        <v>17.30230340426689</v>
       </c>
       <c r="C16" t="n">
-        <v>15.65046805836167</v>
+        <v>15.63374472765234</v>
       </c>
       <c r="D16" t="n">
-        <v>15.18234441802434</v>
+        <v>15.1658840762182</v>
       </c>
       <c r="E16" t="n">
-        <v>14.73762640487201</v>
+        <v>14.7214294281179</v>
       </c>
       <c r="F16" t="n">
-        <v>14.31557227107492</v>
+        <v>14.29963744841218</v>
       </c>
       <c r="G16" t="n">
-        <v>13.91544058758197</v>
+        <v>13.89975993094914</v>
       </c>
       <c r="H16" t="n">
-        <v>13.53648776893828</v>
+        <v>13.52104983533501</v>
       </c>
       <c r="I16" t="n">
-        <v>13.17796526348625</v>
+        <v>13.16276575722204</v>
       </c>
       <c r="J16" t="n">
-        <v>12.47775578822826</v>
+        <v>12.46305065221908</v>
       </c>
       <c r="K16" t="n">
-        <v>14.80434793855716</v>
+        <v>14.77964047872252</v>
       </c>
     </row>
     <row r="17">
@@ -1027,34 +1027,34 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>17.21546131448709</v>
+        <v>17.16620932604729</v>
       </c>
       <c r="C17" t="n">
-        <v>16.0185096088188</v>
+        <v>16.00107577486694</v>
       </c>
       <c r="D17" t="n">
-        <v>15.54740710855816</v>
+        <v>15.53026989260349</v>
       </c>
       <c r="E17" t="n">
-        <v>15.09802685906876</v>
+        <v>15.08117311599967</v>
       </c>
       <c r="F17" t="n">
-        <v>14.66990653601713</v>
+        <v>14.65332348047074</v>
       </c>
       <c r="G17" t="n">
-        <v>14.2773920694733</v>
+        <v>14.26106214382601</v>
       </c>
       <c r="H17" t="n">
-        <v>13.9269103763357</v>
+        <v>13.91081364662703</v>
       </c>
       <c r="I17" t="n">
-        <v>13.59542854532651</v>
+        <v>13.57955419191072</v>
       </c>
       <c r="J17" t="n">
-        <v>13.01668448354246</v>
+        <v>13.0008867317437</v>
       </c>
       <c r="K17" t="n">
-        <v>15.5774044523795</v>
+        <v>15.55068751431124</v>
       </c>
     </row>
     <row r="18">
@@ -1064,34 +1064,34 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>9.0990706824992</v>
+        <v>9.100095945018122</v>
       </c>
       <c r="C18" t="n">
-        <v>8.573315535600671</v>
+        <v>8.567145125953481</v>
       </c>
       <c r="D18" t="n">
-        <v>8.326058417262869</v>
+        <v>8.318705261110853</v>
       </c>
       <c r="E18" t="n">
-        <v>8.087858283084257</v>
+        <v>8.079591769278982</v>
       </c>
       <c r="F18" t="n">
-        <v>7.858798754615956</v>
+        <v>7.849855194065776</v>
       </c>
       <c r="G18" t="n">
-        <v>7.670761735098397</v>
+        <v>7.659702948137785</v>
       </c>
       <c r="H18" t="n">
-        <v>7.539126744545863</v>
+        <v>7.523670832374512</v>
       </c>
       <c r="I18" t="n">
-        <v>7.415883050625482</v>
+        <v>7.396193354346611</v>
       </c>
       <c r="J18" t="n">
-        <v>7.167230161245784</v>
+        <v>7.134897818327829</v>
       </c>
       <c r="K18" t="n">
-        <v>8.33298574442793</v>
+        <v>8.303131772822105</v>
       </c>
     </row>
     <row r="19">
@@ -1101,34 +1101,34 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2.000000000002075</v>
+        <v>1.99999999997838</v>
       </c>
       <c r="C19" t="n">
-        <v>2.119999999999939</v>
+        <v>2.120000000011354</v>
       </c>
       <c r="D19" t="n">
-        <v>2.119999999999919</v>
+        <v>2.120000000000585</v>
       </c>
       <c r="E19" t="n">
-        <v>2.119999999999893</v>
+        <v>2.120000000000123</v>
       </c>
       <c r="F19" t="n">
-        <v>2.119999999999993</v>
+        <v>2.12000000000002</v>
       </c>
       <c r="G19" t="n">
-        <v>2.119999999999797</v>
+        <v>2.120000000000012</v>
       </c>
       <c r="H19" t="n">
-        <v>2.119999999999731</v>
+        <v>2.120000000000016</v>
       </c>
       <c r="I19" t="n">
-        <v>2.119999999999751</v>
+        <v>2.120000000000026</v>
       </c>
       <c r="J19" t="n">
-        <v>2.12000000000008</v>
+        <v>2.120000000000017</v>
       </c>
       <c r="K19" t="n">
-        <v>1.759999999999868</v>
+        <v>1.760000000010415</v>
       </c>
     </row>
     <row r="20">
@@ -1138,34 +1138,34 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.2233475399110565</v>
+        <v>0.2296064874682811</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2385484468662515</v>
+        <v>0.2450747733348159</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2383678069011548</v>
+        <v>0.2448723215702357</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2381968902175597</v>
+        <v>0.2446808965583268</v>
       </c>
       <c r="F20" t="n">
-        <v>0.238035299851671</v>
+        <v>0.244500038636872</v>
       </c>
       <c r="G20" t="n">
-        <v>0.2378826007857454</v>
+        <v>0.2443278300019649</v>
       </c>
       <c r="H20" t="n">
-        <v>0.2377384424311815</v>
+        <v>0.2441631498797155</v>
       </c>
       <c r="I20" t="n">
-        <v>0.2376025506616394</v>
+        <v>0.2440078004336775</v>
       </c>
       <c r="J20" t="n">
-        <v>0.2383381228514234</v>
+        <v>0.2446989847828288</v>
       </c>
       <c r="K20" t="n">
-        <v>0.2018347472917207</v>
+        <v>0.2071529920507962</v>
       </c>
     </row>
     <row r="21">
@@ -1175,34 +1175,34 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.789652460091018</v>
+        <v>1.783393512510098</v>
       </c>
       <c r="C21" t="n">
-        <v>1.897451553133688</v>
+        <v>1.890925226676538</v>
       </c>
       <c r="D21" t="n">
-        <v>1.897632193098765</v>
+        <v>1.89112767843035</v>
       </c>
       <c r="E21" t="n">
-        <v>1.897803109782333</v>
+        <v>1.891319103441796</v>
       </c>
       <c r="F21" t="n">
-        <v>1.897964700148322</v>
+        <v>1.891499961363148</v>
       </c>
       <c r="G21" t="n">
-        <v>1.898117399214051</v>
+        <v>1.891672169998047</v>
       </c>
       <c r="H21" t="n">
-        <v>1.89826155756855</v>
+        <v>1.8918368501203</v>
       </c>
       <c r="I21" t="n">
-        <v>1.898397449338111</v>
+        <v>1.891992199566349</v>
       </c>
       <c r="J21" t="n">
-        <v>1.898661877148657</v>
+        <v>1.892301015217188</v>
       </c>
       <c r="K21" t="n">
-        <v>1.576165252708147</v>
+        <v>1.570847007959618</v>
       </c>
     </row>
     <row r="22">
@@ -1212,34 +1212,34 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.79261765421179</v>
+        <v>1.786359045506833</v>
       </c>
       <c r="C22" t="n">
-        <v>1.90044468863809</v>
+        <v>1.893918641626515</v>
       </c>
       <c r="D22" t="n">
-        <v>1.900633151045768</v>
+        <v>1.894128911433072</v>
       </c>
       <c r="E22" t="n">
-        <v>1.900811499059055</v>
+        <v>1.894327763373149</v>
       </c>
       <c r="F22" t="n">
-        <v>1.900980142036715</v>
+        <v>1.894515669525717</v>
       </c>
       <c r="G22" t="n">
-        <v>1.90113952738553</v>
+        <v>1.894694560196804</v>
       </c>
       <c r="H22" t="n">
-        <v>1.901290018119762</v>
+        <v>1.894865568642563</v>
       </c>
       <c r="I22" t="n">
-        <v>1.901431900874595</v>
+        <v>1.895026905089326</v>
       </c>
       <c r="J22" t="n">
-        <v>1.901708029329602</v>
+        <v>1.895347413124109</v>
       </c>
       <c r="K22" t="n">
-        <v>1.57917252705447</v>
+        <v>1.57385469517074</v>
       </c>
     </row>
     <row r="23">
@@ -1249,34 +1249,34 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.2234064787626266</v>
+        <v>0.2296654433012009</v>
       </c>
       <c r="C23" t="n">
-        <v>0.23860764503479</v>
+        <v>0.2451339960098267</v>
       </c>
       <c r="D23" t="n">
-        <v>0.238427072763443</v>
+        <v>0.2449316084384918</v>
       </c>
       <c r="E23" t="n">
-        <v>0.2382562309503555</v>
+        <v>0.2447402477264404</v>
       </c>
       <c r="F23" t="n">
-        <v>0.2380947023630142</v>
+        <v>0.2445594519376755</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2379420548677444</v>
+        <v>0.244387298822403</v>
       </c>
       <c r="H23" t="n">
-        <v>0.2377979606389999</v>
+        <v>0.2442226856946945</v>
       </c>
       <c r="I23" t="n">
-        <v>0.2376621216535568</v>
+        <v>0.2440673857927322</v>
       </c>
       <c r="J23" t="n">
-        <v>0.2383978068828583</v>
+        <v>0.2447586804628372</v>
       </c>
       <c r="K23" t="n">
-        <v>0.2018941342830658</v>
+        <v>0.2072123885154724</v>
       </c>
     </row>
     <row r="24">
@@ -1323,34 +1323,34 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1.016024112701416</v>
+        <v>1.016024470329285</v>
       </c>
       <c r="C25" t="n">
-        <v>1.079052329063416</v>
+        <v>1.079052686691284</v>
       </c>
       <c r="D25" t="n">
-        <v>1.079060196876526</v>
+        <v>1.079060554504395</v>
       </c>
       <c r="E25" t="n">
-        <v>1.079067707061768</v>
+        <v>1.079068064689636</v>
       </c>
       <c r="F25" t="n">
-        <v>1.079074859619141</v>
+        <v>1.07907509803772</v>
       </c>
       <c r="G25" t="n">
-        <v>1.079081535339355</v>
+        <v>1.079081892967224</v>
       </c>
       <c r="H25" t="n">
-        <v>1.079087972640991</v>
+        <v>1.07908821105957</v>
       </c>
       <c r="I25" t="n">
-        <v>1.079094052314758</v>
+        <v>1.079094290733337</v>
       </c>
       <c r="J25" t="n">
-        <v>1.080105781555176</v>
+        <v>1.080106139183044</v>
       </c>
       <c r="K25" t="n">
-        <v>0.9010666608810425</v>
+        <v>0.9010670781135559</v>
       </c>
     </row>
     <row r="26">
@@ -1360,34 +1360,34 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.1175354123785345</v>
+        <v>0.1214574831347294</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1172880785802975</v>
+        <v>0.1211442790561498</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1171817213629983</v>
+        <v>0.1210242566806496</v>
       </c>
       <c r="E26" t="n">
-        <v>0.1170811076619242</v>
+        <v>0.1209107950859146</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1169860007587704</v>
+        <v>0.1208036179245803</v>
       </c>
       <c r="G26" t="n">
-        <v>0.1168961418706871</v>
+        <v>0.1207015854138197</v>
       </c>
       <c r="H26" t="n">
-        <v>0.1168113222053564</v>
+        <v>0.1206040308735961</v>
       </c>
       <c r="I26" t="n">
-        <v>0.1167313782152956</v>
+        <v>0.1205120192810191</v>
       </c>
       <c r="J26" t="n">
-        <v>0.1165758503477308</v>
+        <v>0.120329156382498</v>
       </c>
       <c r="K26" t="n">
-        <v>0.1166341834879676</v>
+        <v>0.1204146496077222</v>
       </c>
     </row>
     <row r="27">
@@ -1471,34 +1471,34 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>104.7979765625</v>
+        <v>104.5764609375</v>
       </c>
       <c r="C29" t="n">
-        <v>100.1004375</v>
+        <v>99.853296875</v>
       </c>
       <c r="D29" t="n">
-        <v>97.0497109375</v>
+        <v>96.79503124999999</v>
       </c>
       <c r="E29" t="n">
-        <v>94.17159375</v>
+        <v>93.9093125</v>
       </c>
       <c r="F29" t="n">
-        <v>91.458546875</v>
+        <v>91.18864062500001</v>
       </c>
       <c r="G29" t="n">
-        <v>88.9036171875</v>
+        <v>88.62642187500001</v>
       </c>
       <c r="H29" t="n">
-        <v>86.499921875</v>
+        <v>86.216046875</v>
       </c>
       <c r="I29" t="n">
-        <v>84.2400390625</v>
+        <v>83.94959375000001</v>
       </c>
       <c r="J29" t="n">
-        <v>79.9013203125</v>
+        <v>79.5993359375</v>
       </c>
       <c r="K29" t="n">
-        <v>78.7936015625</v>
+        <v>78.571546875</v>
       </c>
     </row>
     <row r="30">
@@ -1508,34 +1508,34 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>100.145734375</v>
+        <v>100.1463671875</v>
       </c>
       <c r="C30" t="n">
-        <v>94.8716015625</v>
+        <v>94.8722578125</v>
       </c>
       <c r="D30" t="n">
-        <v>91.72541406249999</v>
+        <v>91.7260625</v>
       </c>
       <c r="E30" t="n">
-        <v>88.75129687499999</v>
+        <v>88.7519453125</v>
       </c>
       <c r="F30" t="n">
-        <v>85.94196875</v>
+        <v>85.942609375</v>
       </c>
       <c r="G30" t="n">
-        <v>83.2903359375</v>
+        <v>83.29098437499999</v>
       </c>
       <c r="H30" t="n">
-        <v>80.789546875</v>
+        <v>80.7901875</v>
       </c>
       <c r="I30" t="n">
-        <v>78.4329453125</v>
+        <v>78.4335859375</v>
       </c>
       <c r="J30" t="n">
-        <v>73.88982812499999</v>
+        <v>73.89046875</v>
       </c>
       <c r="K30" t="n">
-        <v>74.2820859375</v>
+        <v>74.28261718749999</v>
       </c>
     </row>
     <row r="31">
@@ -1545,34 +1545,34 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>104.7979746794885</v>
+        <v>104.5764627205822</v>
       </c>
       <c r="C31" t="n">
-        <v>100.100439497793</v>
+        <v>99.85329808712335</v>
       </c>
       <c r="D31" t="n">
-        <v>97.04971460705875</v>
+        <v>96.79502769967377</v>
       </c>
       <c r="E31" t="n">
-        <v>94.17159256227755</v>
+        <v>93.90931025889061</v>
       </c>
       <c r="F31" t="n">
-        <v>91.4585465942038</v>
+        <v>91.18863749321415</v>
       </c>
       <c r="G31" t="n">
-        <v>88.90361460499103</v>
+        <v>88.62642336877202</v>
       </c>
       <c r="H31" t="n">
-        <v>86.4999181146412</v>
+        <v>86.21604365114661</v>
       </c>
       <c r="I31" t="n">
-        <v>84.24003954140935</v>
+        <v>83.94959077244501</v>
       </c>
       <c r="J31" t="n">
-        <v>79.90132142658987</v>
+        <v>79.59933254962218</v>
       </c>
       <c r="K31" t="n">
-        <v>78.79359898399856</v>
+        <v>78.57154913463265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>